<commit_message>
GFRA3+C switched to novel
</commit_message>
<xml_diff>
--- a/evaluation/WTC11/WTC11.RT-PCR_Support.xlsx
+++ b/evaluation/WTC11/WTC11.RT-PCR_Support.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markd/compbio/gencode/projs/lrgasp/experimental-eval/evaluation/WTC11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46B91F9-CB0A-6143-A5BA-08D27A4F0844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E770A963-05DE-834A-A649-98CE3C3EF849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -3244,6 +3244,14 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
@@ -3263,10 +3271,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
+          <fgColor rgb="FFFF6D01"/>
+          <bgColor rgb="FFFF6D01"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3275,17 +3286,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF6D01"/>
-          <bgColor rgb="FFFF6D01"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3309,6 +3309,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
@@ -3328,10 +3336,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
+          <fgColor rgb="FFFF6D01"/>
+          <bgColor rgb="FFFF6D01"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3340,17 +3351,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF6D01"/>
-          <bgColor rgb="FFFF6D01"/>
         </patternFill>
       </fill>
     </dxf>
@@ -22850,20 +22850,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M269">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"investigate"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"unsupported"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
-      <formula>"investigate"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
-      <formula>"end exon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"likely"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"supported"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"end exon"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" gridLines="1"/>
@@ -22880,10 +22880,10 @@
   <dimension ref="A1:S239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="O31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1:Q1048576"/>
+      <selection pane="bottomRight" activeCell="N107" sqref="N107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -28462,7 +28462,7 @@
         <v>257</v>
       </c>
       <c r="M105" s="13" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="N105" s="13" t="s">
         <v>75</v>
@@ -28517,7 +28517,7 @@
         <v>6</v>
       </c>
       <c r="M106" s="6" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="N106" s="6"/>
       <c r="O106" s="10"/>
@@ -28570,7 +28570,7 @@
         <v>1</v>
       </c>
       <c r="M107" s="6" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="N107" s="6"/>
       <c r="O107" s="10"/>
@@ -35585,6 +35585,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="O69:O71"/>
+    <mergeCell ref="O78:O80"/>
+    <mergeCell ref="O87:O89"/>
+    <mergeCell ref="O90:O92"/>
+    <mergeCell ref="O111:O113"/>
     <mergeCell ref="O48:O50"/>
     <mergeCell ref="O60:O62"/>
     <mergeCell ref="F1:G1"/>
@@ -35592,11 +35597,6 @@
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="O39:O41"/>
     <mergeCell ref="O45:O47"/>
-    <mergeCell ref="O69:O71"/>
-    <mergeCell ref="O78:O80"/>
-    <mergeCell ref="O87:O89"/>
-    <mergeCell ref="O90:O92"/>
-    <mergeCell ref="O111:O113"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:S239">
     <cfRule type="expression" dxfId="6" priority="7">
@@ -35609,20 +35609,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N239">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"investigate"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"unsupported"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"investigate"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"end exon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"likely"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"supported"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"end exon"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>